<commit_message>
Add info in How_to_Install_Project_2_Apps.xlsx(3)
</commit_message>
<xml_diff>
--- a/How_to_Install_Project_2_Apps.xlsx
+++ b/How_to_Install_Project_2_Apps.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Step1: download zip file</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Step 7. Open cmd - Command Prompt</t>
-  </si>
-  <si>
-    <t>Step 8 run command</t>
   </si>
   <si>
     <t>OR</t>
@@ -129,12 +126,84 @@
       <t>node server.js</t>
     </r>
   </si>
+  <si>
+    <t>https://www.tutorialspoint.com/angular/angular-environment-setup.htm</t>
+  </si>
+  <si>
+    <t>Open cmd, run command: npm install express cors --save</t>
+  </si>
+  <si>
+    <t>0.1 Install Node.js and Angular</t>
+  </si>
+  <si>
+    <r>
+      <t>0.2 Install </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>express</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t> packages to create node-based web applications</t>
+    </r>
+  </si>
+  <si>
+    <t>0.3 Install SQLite package</t>
+  </si>
+  <si>
+    <t>Open cmd, run command: npm install sqlite3 --save</t>
+  </si>
+  <si>
+    <t>0.4 Download SQLiteStudio installer file and install it</t>
+  </si>
+  <si>
+    <t>https://sqlitestudio.pl/</t>
+  </si>
+  <si>
+    <t>Step 8. Run command</t>
+  </si>
+  <si>
+    <t>Step 9. Open SQLiteStudio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +234,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,11 +276,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -214,13 +306,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>474592</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>161075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -257,13 +349,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>180190</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>180714</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -300,13 +392,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>36724</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>151976</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -343,13 +435,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>113448</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>161690</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -386,13 +478,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -446,13 +538,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>142876</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -506,13 +598,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -566,13 +658,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -626,13 +718,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>314326</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -686,13 +778,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -746,13 +838,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>84952</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>161762</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -789,13 +881,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>237258</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>47095</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -832,13 +924,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>494401</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>66405</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -875,13 +967,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>504824</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -935,13 +1027,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>314324</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -995,13 +1087,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>107</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1055,13 +1147,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>504824</xdr:colOff>
-      <xdr:row>117</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1115,13 +1207,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1175,13 +1267,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1235,13 +1327,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1299,13 +1391,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1363,13 +1455,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>113219</xdr:colOff>
-      <xdr:row>156</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>113690</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1406,13 +1498,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>131</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>146</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1466,13 +1558,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>148</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1526,13 +1618,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>154</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>156</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1586,13 +1678,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>159</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1646,13 +1738,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>160</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>147</xdr:row>
+      <xdr:row>161</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1706,13 +1798,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>136</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>151</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1770,13 +1862,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>147</xdr:row>
+      <xdr:row>161</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>162</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1834,13 +1926,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>174</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>312152</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>184</xdr:row>
       <xdr:rowOff>123571</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1877,13 +1969,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>172</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>140800</xdr:colOff>
-      <xdr:row>181</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>66452</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1920,13 +2012,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>174</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1980,13 +2072,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>174</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2040,13 +2132,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>181</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2100,13 +2192,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>181</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2160,13 +2252,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>183</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2224,13 +2316,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>163</xdr:row>
+      <xdr:row>177</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2288,13 +2380,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>163</xdr:row>
+      <xdr:row>177</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2352,13 +2444,13 @@
     <xdr:from>
       <xdr:col>27</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>183</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2416,13 +2508,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>181</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2469,13 +2561,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>290512</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>175</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>167</xdr:row>
+      <xdr:row>181</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2522,13 +2614,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>183</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>185</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2586,13 +2678,13 @@
     <xdr:from>
       <xdr:col>27</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>183</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>185</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2650,13 +2742,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>178</xdr:row>
+      <xdr:row>192</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2710,13 +2802,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>178</xdr:row>
+      <xdr:row>192</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2770,13 +2862,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>185</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2823,13 +2915,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>185</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>177</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2876,13 +2968,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2936,13 +3028,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>188</xdr:row>
+      <xdr:row>202</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>150324</xdr:colOff>
-      <xdr:row>207</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>123357</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2979,13 +3071,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>191</xdr:row>
+      <xdr:row>205</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>206</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3039,13 +3131,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>202</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3099,13 +3191,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>323851</xdr:colOff>
-      <xdr:row>191</xdr:row>
+      <xdr:row>205</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>247651</xdr:colOff>
-      <xdr:row>192</xdr:row>
+      <xdr:row>206</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3159,13 +3251,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>194</xdr:row>
+      <xdr:row>208</xdr:row>
       <xdr:rowOff>114297</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>195</xdr:row>
+      <xdr:row>209</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3219,13 +3311,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>198</xdr:row>
+      <xdr:row>212</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>199</xdr:row>
+      <xdr:row>213</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3279,13 +3371,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3339,13 +3431,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3399,13 +3491,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3459,13 +3551,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3519,13 +3611,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3583,13 +3675,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3647,13 +3739,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>133351</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>285751</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3711,13 +3803,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3775,13 +3867,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>198</xdr:row>
+      <xdr:row>212</xdr:row>
       <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>437029</xdr:colOff>
-      <xdr:row>199</xdr:row>
+      <xdr:row>213</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3839,13 +3931,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>202</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>204</xdr:row>
+      <xdr:row>218</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3903,13 +3995,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>210</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>244</xdr:row>
+      <xdr:row>258</xdr:row>
       <xdr:rowOff>31056</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3946,13 +4038,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>210</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>189867</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>85548</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3989,13 +4081,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
       <xdr:colOff>178743</xdr:colOff>
-      <xdr:row>232</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>75845</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4032,13 +4124,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>361951</xdr:colOff>
-      <xdr:row>210</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>211</xdr:row>
+      <xdr:row>225</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4092,13 +4184,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>210</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>211</xdr:row>
+      <xdr:row>225</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4152,13 +4244,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>219</xdr:row>
+      <xdr:row>233</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4206,6 +4298,1019 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>272157</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612913" y="1358348"/>
+          <a:ext cx="2723809" cy="438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>446975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612913" y="2310848"/>
+          <a:ext cx="2285714" cy="390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>543026</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>104000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612913" y="49745348"/>
+          <a:ext cx="9123809" cy="6200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>461347</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>123567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9763125" y="49710975"/>
+          <a:ext cx="6547822" cy="2066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>272</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>36810</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>56713</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9772650" y="52025550"/>
+          <a:ext cx="3675360" cy="3495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>17905</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>189833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="56607075"/>
+          <a:ext cx="9161905" cy="5333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="Rectangle 100"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600076" y="50015774"/>
+          <a:ext cx="685800" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="Rectangle 101"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266824" y="50177700"/>
+          <a:ext cx="1152525" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Click</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Database</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>565288</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>43898</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>269</xdr:row>
+      <xdr:rowOff>167723</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="103" name="Rectangle 102"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1174888" y="51126473"/>
+          <a:ext cx="1520687" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Select Add a Databse</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333376</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>106432</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>43898</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="104" name="Straight Arrow Connector 103"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="101" idx="2"/>
+          <a:endCxn id="103" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="942976" y="50196749"/>
+          <a:ext cx="992256" cy="929724"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>269</xdr:row>
+      <xdr:rowOff>10561</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>269</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="105" name="Straight Arrow Connector 104"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="103" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2695575" y="51283636"/>
+          <a:ext cx="923925" cy="8489"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>278</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="106" name="Rectangle 105"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6724650" y="52739925"/>
+          <a:ext cx="257175" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="107" name="Rectangle 106"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3686175" y="52273200"/>
+          <a:ext cx="1695450" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>277</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="108" name="Straight Arrow Connector 107"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="106" idx="3"/>
+          <a:endCxn id="110" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6981825" y="50601563"/>
+          <a:ext cx="2981325" cy="2271712"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="109" name="Rectangle 108"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11649075" y="49710975"/>
+          <a:ext cx="1981200" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="Rectangle 109"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9963150" y="50511075"/>
+          <a:ext cx="809625" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>27930</xdr:colOff>
+      <xdr:row>272</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="111" name="Straight Arrow Connector 110"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="110" idx="3"/>
+          <a:endCxn id="35" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10772775" y="50601563"/>
+          <a:ext cx="837555" cy="1423987"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>289</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="112" name="Rectangle 111"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11772900" y="55121175"/>
+          <a:ext cx="752475" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>313753</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>566738</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="113" name="Straight Arrow Connector 112"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="112" idx="2"/>
+          <a:endCxn id="36" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5190553" y="55387875"/>
+          <a:ext cx="6958585" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4474,23 +5579,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y187"/>
+  <dimension ref="B2:Y261"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -4499,86 +5604,225 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>2</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G72" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>5</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C106" t="s">
         <v>6</v>
       </c>
-      <c r="N92" t="s">
+      <c r="N106" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B184" t="s">
+    <row r="198" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="199" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B199" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q199" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q200" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y200" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B185" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q185" s="2" t="s">
-        <v>13</v>
+    <row r="201" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="Q201" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="186" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q186" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y186" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="187" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="Q187" t="s">
-        <v>20</v>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>